<commit_message>
changes committed to excel
</commit_message>
<xml_diff>
--- a/DSA.xlsx
+++ b/DSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G3\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9535F1F0-6387-4B6F-9098-F4D2A55F12F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0EC67B-2089-495D-B905-F54665F77B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="490">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1492,6 +1492,9 @@
   </si>
   <si>
     <t>Eureka!, TLE</t>
+  </si>
+  <si>
+    <t>1 test case, needs optimization</t>
   </si>
 </sst>
 </file>
@@ -1751,9 +1754,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE2A51C"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFEA0000"/>
-      <color rgb="FFE2A51C"/>
       <color rgb="FF0066FF"/>
     </mruColors>
   </colors>
@@ -2068,7 +2071,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="B439" sqref="B439"/>
+      <selection activeCell="B442" sqref="B442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -6605,8 +6608,8 @@
       </c>
     </row>
     <row r="439" spans="1:3" ht="21">
-      <c r="A439" s="5" t="s">
-        <v>393</v>
+      <c r="A439" s="32" t="s">
+        <v>482</v>
       </c>
       <c r="B439" s="6" t="s">
         <v>422</v>
@@ -6616,18 +6619,18 @@
       </c>
     </row>
     <row r="440" spans="1:3" ht="21">
-      <c r="A440" s="5" t="s">
+      <c r="A440" s="17" t="s">
         <v>393</v>
       </c>
       <c r="B440" s="6" t="s">
         <v>423</v>
       </c>
       <c r="C440" s="4" t="s">
-        <v>4</v>
+        <v>489</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="21">
-      <c r="A441" s="5" t="s">
+      <c r="A441" s="17" t="s">
         <v>393</v>
       </c>
       <c r="B441" s="6" t="s">

</xml_diff>